<commit_message>
excel ranges in io excel factory updated, ranges are now in line with their tab
</commit_message>
<xml_diff>
--- a/web/files/xml_storage/simpel rekenmodel.xlsx
+++ b/web/files/xml_storage/simpel rekenmodel.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="75">
   <si>
     <t>Persoon</t>
   </si>
@@ -44,6 +44,33 @@
   </si>
   <si>
     <t>Studerend</t>
+  </si>
+  <si>
+    <t>20-05-1986</t>
+  </si>
+  <si>
+    <t>Ruben Hazenbosch</t>
+  </si>
+  <si>
+    <t>Man</t>
+  </si>
+  <si>
+    <t>Karin</t>
+  </si>
+  <si>
+    <t>dfdfdf</t>
+  </si>
+  <si>
+    <t>11-05-2001</t>
+  </si>
+  <si>
+    <t>Pietje</t>
+  </si>
+  <si>
+    <t>Onbekend</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
   <si>
     <t>Soort</t>
@@ -633,7 +660,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -670,6 +697,15 @@
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
@@ -682,13 +718,35 @@
     </row>
     <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
@@ -737,7 +795,6 @@
     </row>
     <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -747,14 +804,12 @@
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -764,12 +819,10 @@
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -779,14 +832,12 @@
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -797,7 +848,6 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
@@ -847,7 +897,7 @@
   <dimension ref="A2:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -857,70 +907,60 @@
   <sheetData>
     <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-    </row>
+    <row r="5" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
@@ -996,7 +1036,7 @@
     </row>
     <row r="28" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B28">
         <v>300</v>
@@ -1004,7 +1044,7 @@
     </row>
     <row r="29" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B29">
         <v>400</v>
@@ -1012,18 +1052,18 @@
     </row>
     <row r="30" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B30">
         <v>900</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B31">
         <v>330</v>
@@ -1031,7 +1071,7 @@
     </row>
     <row r="32" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B32">
         <v>440</v>
@@ -1039,13 +1079,13 @@
     </row>
     <row r="33" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B33">
         <v>990</v>
       </c>
       <c r="D33" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1078,36 +1118,36 @@
   <sheetData>
     <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B3" s="5" t="str">
         <f>'Input Oud'!B3</f>
         <v>Piet</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B4" s="5">
         <f>YEAR('Input Oud'!B19)-YEAR('Input Oud'!B4)+(MONTH('Input Oud'!B19)-MONTH('Input Oud'!B4))/12</f>
         <v>-70.083333333333329</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B5" s="5">
         <v>67</v>
@@ -1115,7 +1155,7 @@
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B6" s="5">
         <v>20</v>
@@ -1123,7 +1163,7 @@
     </row>
     <row r="7" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B7" s="5">
         <v>450</v>
@@ -1131,7 +1171,7 @@
     </row>
     <row r="8" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B8" s="5">
         <v>1082</v>
@@ -1139,7 +1179,7 @@
     </row>
     <row r="9" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B9" s="5">
         <f>'Input Oud'!B12-(YEAR('Input Oud'!B19)-YEAR('Input Oud'!B11)+(MONTH('Input Oud'!B19)-MONTH('Input Oud'!B11))/12)</f>
@@ -1148,21 +1188,21 @@
     </row>
     <row r="11" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1179,7 +1219,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1196,7 +1236,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1213,7 +1253,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1230,7 +1270,7 @@
         <v>1082</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1260,7 +1300,7 @@
   <sheetData>
     <row r="3" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B3" s="8">
         <v>18202</v>
@@ -1271,7 +1311,7 @@
     </row>
     <row r="4" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B4" s="8">
         <v>18536</v>
@@ -1282,7 +1322,7 @@
     </row>
     <row r="5" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B5" s="8">
         <v>18810</v>
@@ -1293,7 +1333,7 @@
     </row>
     <row r="6" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B6" s="8">
         <v>19085</v>
@@ -1304,7 +1344,7 @@
     </row>
     <row r="7" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B7" s="8">
         <v>19359</v>
@@ -1315,7 +1355,7 @@
     </row>
     <row r="8" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B8" s="8">
         <v>19603</v>
@@ -1326,7 +1366,7 @@
     </row>
     <row r="9" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B9" s="8">
         <v>19845</v>
@@ -1337,7 +1377,7 @@
     </row>
     <row r="10" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B10" s="8">
         <v>43831</v>
@@ -1348,32 +1388,32 @@
     </row>
     <row r="11" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1410,19 +1450,19 @@
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1437,7 +1477,7 @@
         <v>Persoon moet ouder zijn dan 65</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1445,19 +1485,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C5" s="11" t="str">
         <f>IF(OR(B5="M",B5="V",B5="onbekend"),"","Geslacht is M, V of onbekend")</f>
         <v/>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B6" s="5">
         <f>2016-YEAR(B4)+(8-MONTH(B4))/12+(1-DAY(B4))/365</f>
@@ -1467,92 +1507,92 @@
     </row>
     <row r="8" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>